<commit_message>
replaced data results with new results including aggregate model with factor use
</commit_message>
<xml_diff>
--- a/data/replace.xlsx
+++ b/data/replace.xlsx
@@ -118,94 +118,94 @@
     <t xml:space="preserve">W F Time</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;S:102&gt; = &lt;init&gt; -&gt; &lt;S:102&gt;.equals(\"AC\"){61}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'A'){254} -&gt; &lt;S:18&gt;.equals(\"BC\"){259}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'A'){2569} -&gt; &lt;S:6&gt;.contains(\"A\"){3279}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'A'){286} -&gt; &lt;S:15&gt;.contains(\"D\"){670}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'A'){287} -&gt; &lt;S:21&gt;.equals(\"AC\"){381}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'A'){383} -&gt; &lt;S:12&gt;.contains(\"B\"){1167}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'A'){397} -&gt; &lt;S:9&gt;.contains(\"C\"){1921}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'B'){194} -&gt; &lt;S:33&gt;.contains(\"B\"){698}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'B'){213} -&gt; &lt;S:42&gt;.equals(\"AC\"){268}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'B'){226} -&gt; &lt;S:30&gt;.contains(\"C\"){805}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'B'){235} -&gt; &lt;S:39&gt;.equals(\"BC\"){240}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'B'){253} -&gt; &lt;S:36&gt;.contains(\"D\"){512}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'B'){284} -&gt; &lt;S:27&gt;.contains(\"A\"){698}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'A'){209} -&gt; &lt;S:63&gt;.equals(\"AC\"){214}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'A'){211} -&gt; &lt;S:54&gt;.contains(\"B\"){654}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'A'){215} -&gt; &lt;S:57&gt;.contains(\"D\"){458}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'A'){217} -&gt; &lt;S:60&gt;.equals(\"AC\"){223}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'A'){227} -&gt; &lt;S:51&gt;.contains(\"C\"){830}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'A'){288} -&gt; &lt;S:48&gt;.contains(\"A\"){784}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'B'){165} -&gt; &lt;S:81&gt;.equals(\"BC\"){170}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'B'){172} -&gt; &lt;S:78&gt;.contains(\"D\"){379}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'B'){180} -&gt; &lt;S:75&gt;.contains(\"B\"){629}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'B'){189} -&gt; &lt;S:72&gt;.contains(\"C\"){638}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'B'){192} -&gt; &lt;S:84&gt;.equals(\"AC\"){253}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'B'){202} -&gt; &lt;S:69&gt;.contains(\"A\"){417}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:87&gt; = &lt;init&gt; -&gt; &lt;S:87&gt;.contains(\"A\"){208}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:90&gt; = &lt;init&gt; -&gt; &lt;S:90&gt;.contains(\"C\"){421}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:93&gt; = &lt;init&gt; -&gt; &lt;S:93&gt;.contains(\"B\"){369}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:96&gt; = &lt;init&gt; -&gt; &lt;S:96&gt;.contains(\"D\"){204}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;S:99&gt; = &lt;init&gt; -&gt; &lt;S:99&gt;.equals(\"BC\"){14}</t>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'A'){2759} -&gt; &lt;S:6&gt;.contains(\"A\"){3501}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'A'){413} -&gt; &lt;S:9&gt;.contains(\"C\"){1654}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'A'){342} -&gt; &lt;S:12&gt;.contains(\"B\"){737}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'A'){302} -&gt; &lt;S:15&gt;.contains(\"D\"){625}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'A'){283} -&gt; &lt;S:18&gt;.equals(\"CC\"){288}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'A'){239} -&gt; &lt;S:21&gt;.equals(\"AC\"){324}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'B'){293} -&gt; &lt;S:27&gt;.contains(\"A\"){582}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'B'){231} -&gt; &lt;S:30&gt;.contains(\"C\"){856}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'B'){292} -&gt; &lt;S:33&gt;.contains(\"B\"){598}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'B'){236} -&gt; &lt;S:36&gt;.contains(\"D\"){503}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'B'){225} -&gt; &lt;S:39&gt;.equals(\"CC\"){230}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('A', 'B'){296} -&gt; &lt;S:42&gt;.equals(\"AC\"){352}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'A'){400} -&gt; &lt;S:48&gt;.contains(\"A\"){675}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'A'){218} -&gt; &lt;S:51&gt;.contains(\"C\"){861}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'A'){213} -&gt; &lt;S:54&gt;.contains(\"B\"){433}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'A'){201} -&gt; &lt;S:57&gt;.contains(\"D\"){439}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'A'){228} -&gt; &lt;S:60&gt;.equals(\"CC\"){233}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'A'){246} -&gt; &lt;S:63&gt;.equals(\"AC\"){315}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'B'){206} -&gt; &lt;S:69&gt;.contains(\"A\"){475}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'B'){183} -&gt; &lt;S:72&gt;.contains(\"C\"){609}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'B'){191} -&gt; &lt;S:75&gt;.contains(\"B\"){507}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'B'){267} -&gt; &lt;S:78&gt;.contains(\"D\"){590}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'B'){165} -&gt; &lt;S:81&gt;.equals(\"CC\"){170}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:2&gt; = &lt;init&gt; -&gt; &lt;S:2&gt;.replace('B', 'B'){162} -&gt; &lt;S:84&gt;.equals(\"AC\"){218}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:87&gt; = &lt;init&gt; -&gt; &lt;S:87&gt;.contains(\"A\"){203}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:90&gt; = &lt;init&gt; -&gt; &lt;S:90&gt;.contains(\"C\"){424}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:93&gt; = &lt;init&gt; -&gt; &lt;S:93&gt;.contains(\"B\"){214}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:96&gt; = &lt;init&gt; -&gt; &lt;S:96&gt;.contains(\"D\"){227}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:99&gt; = &lt;init&gt; -&gt; &lt;S:99&gt;.equals(\"CC\"){15}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;S:102&gt; = &lt;init&gt; -&gt; &lt;S:102&gt;.equals(\"AC\"){57}</t>
   </si>
 </sst>
 </file>
@@ -303,8 +303,8 @@
   </sheetPr>
   <dimension ref="A1:AF31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M:M"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -438,7 +438,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>32</v>
@@ -459,84 +459,84 @@
         <v>85</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="O2" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="P2" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="R2" s="0" t="n">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="S2" s="0" t="n">
-        <v>61</v>
+        <v>3501</v>
       </c>
       <c r="T2" s="0" t="n">
-        <v>65</v>
+        <v>3696</v>
       </c>
       <c r="U2" s="0" t="n">
-        <v>1223</v>
+        <v>10276</v>
       </c>
       <c r="V2" s="0" t="n">
-        <v>206668</v>
+        <v>218146</v>
       </c>
       <c r="W2" s="0" t="n">
-        <v>21</v>
+        <v>110</v>
       </c>
       <c r="X2" s="0" t="n">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="Y2" s="0" t="n">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="Z2" s="0" t="n">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="AA2" s="0" t="n">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="AB2" s="0" t="n">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="AC2" s="0" t="n">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="AD2" s="0" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="AE2" s="0" t="n">
-        <v>15</v>
+        <v>101</v>
       </c>
       <c r="AF2" s="0" t="n">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>33</v>
@@ -557,84 +557,84 @@
         <v>85</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="Q3" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="R3" s="0" t="n">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="S3" s="0" t="n">
-        <v>259</v>
+        <v>1654</v>
       </c>
       <c r="T3" s="0" t="n">
-        <v>833</v>
+        <v>2378</v>
       </c>
       <c r="U3" s="0" t="n">
-        <v>5866</v>
+        <v>5421</v>
       </c>
       <c r="V3" s="0" t="n">
-        <v>1339</v>
+        <v>3286</v>
       </c>
       <c r="W3" s="0" t="n">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="X3" s="0" t="n">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="Y3" s="0" t="n">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Z3" s="0" t="n">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="AA3" s="0" t="n">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="AB3" s="0" t="n">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AC3" s="0" t="n">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="AD3" s="0" t="n">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="AE3" s="0" t="n">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="AF3" s="0" t="n">
-        <v>51</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>34</v>
@@ -685,49 +685,49 @@
         <v>40</v>
       </c>
       <c r="R4" s="0" t="n">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="S4" s="0" t="n">
-        <v>3279</v>
+        <v>737</v>
       </c>
       <c r="T4" s="0" t="n">
-        <v>4233</v>
+        <v>845</v>
       </c>
       <c r="U4" s="0" t="n">
-        <v>10159</v>
+        <v>3399</v>
       </c>
       <c r="V4" s="0" t="n">
-        <v>253744</v>
+        <v>227367</v>
       </c>
       <c r="W4" s="0" t="n">
-        <v>127</v>
+        <v>35</v>
       </c>
       <c r="X4" s="0" t="n">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="Y4" s="0" t="n">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="Z4" s="0" t="n">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="AA4" s="0" t="n">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="AB4" s="0" t="n">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="AC4" s="0" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="AD4" s="0" t="n">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="AE4" s="0" t="n">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="AF4" s="0" t="n">
-        <v>42</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,54 +783,54 @@
         <v>40</v>
       </c>
       <c r="R5" s="0" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="S5" s="0" t="n">
-        <v>670</v>
+        <v>625</v>
       </c>
       <c r="T5" s="0" t="n">
-        <v>700</v>
+        <v>704</v>
       </c>
       <c r="U5" s="0" t="n">
-        <v>3298</v>
+        <v>2426</v>
       </c>
       <c r="V5" s="0" t="n">
-        <v>224285</v>
+        <v>208133</v>
       </c>
       <c r="W5" s="0" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X5" s="0" t="n">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="Y5" s="0" t="n">
         <v>46</v>
       </c>
       <c r="Z5" s="0" t="n">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="AA5" s="0" t="n">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="AB5" s="0" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="AC5" s="0" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="AD5" s="0" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="AE5" s="0" t="n">
         <v>51</v>
       </c>
       <c r="AF5" s="0" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>36</v>
@@ -881,54 +881,54 @@
         <v>84</v>
       </c>
       <c r="R6" s="0" t="n">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="S6" s="0" t="n">
-        <v>381</v>
+        <v>288</v>
       </c>
       <c r="T6" s="0" t="n">
-        <v>644</v>
+        <v>385</v>
       </c>
       <c r="U6" s="0" t="n">
-        <v>2429</v>
+        <v>1952</v>
       </c>
       <c r="V6" s="0" t="n">
-        <v>336203</v>
+        <v>936</v>
       </c>
       <c r="W6" s="0" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="X6" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y6" s="0" t="n">
         <v>18</v>
       </c>
       <c r="Z6" s="0" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="AA6" s="0" t="n">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="AB6" s="0" t="n">
         <v>33</v>
       </c>
       <c r="AC6" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="AD6" s="0" t="n">
         <v>50</v>
-      </c>
-      <c r="AD6" s="0" t="n">
-        <v>54</v>
       </c>
       <c r="AE6" s="0" t="n">
         <v>74</v>
       </c>
       <c r="AF6" s="0" t="n">
-        <v>103</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>37</v>
@@ -949,84 +949,84 @@
         <v>85</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="M7" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="N7" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="O7" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="P7" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Q7" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="R7" s="0" t="n">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="S7" s="0" t="n">
-        <v>1167</v>
+        <v>324</v>
       </c>
       <c r="T7" s="0" t="n">
-        <v>1719</v>
+        <v>438</v>
       </c>
       <c r="U7" s="0" t="n">
-        <v>4031</v>
+        <v>3467</v>
       </c>
       <c r="V7" s="0" t="n">
-        <v>3149</v>
+        <v>332617</v>
       </c>
       <c r="W7" s="0" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="X7" s="0" t="n">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="Y7" s="0" t="n">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="Z7" s="0" t="n">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="AA7" s="0" t="n">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="AB7" s="0" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AC7" s="0" t="n">
         <v>48</v>
       </c>
       <c r="AD7" s="0" t="n">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AE7" s="0" t="n">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="AF7" s="0" t="n">
-        <v>92</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>38</v>
@@ -1035,34 +1035,34 @@
         <v>85</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>85</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="M8" s="0" t="n">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="N8" s="0" t="n">
         <v>40</v>
@@ -1074,57 +1074,57 @@
         <v>40</v>
       </c>
       <c r="Q8" s="0" t="n">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="R8" s="0" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S8" s="0" t="n">
-        <v>1921</v>
+        <v>582</v>
       </c>
       <c r="T8" s="0" t="n">
-        <v>2531</v>
+        <v>646</v>
       </c>
       <c r="U8" s="0" t="n">
-        <v>4176</v>
+        <v>2263</v>
       </c>
       <c r="V8" s="0" t="n">
-        <v>4162</v>
+        <v>218103</v>
       </c>
       <c r="W8" s="0" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="X8" s="0" t="n">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="Y8" s="0" t="n">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="Z8" s="0" t="n">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="AA8" s="0" t="n">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="AB8" s="0" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AC8" s="0" t="n">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="AD8" s="0" t="n">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="AE8" s="0" t="n">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="AF8" s="0" t="n">
-        <v>96</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>39</v>
@@ -1145,7 +1145,7 @@
         <v>85</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>25</v>
@@ -1157,10 +1157,10 @@
         <v>25</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="M9" s="0" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>15</v>
@@ -1172,57 +1172,57 @@
         <v>15</v>
       </c>
       <c r="Q9" s="0" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="R9" s="0" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S9" s="0" t="n">
-        <v>698</v>
+        <v>856</v>
       </c>
       <c r="T9" s="0" t="n">
-        <v>1281</v>
+        <v>1513</v>
       </c>
       <c r="U9" s="0" t="n">
-        <v>1925</v>
+        <v>2925</v>
       </c>
       <c r="V9" s="0" t="n">
-        <v>2462</v>
+        <v>4005</v>
       </c>
       <c r="W9" s="0" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="X9" s="0" t="n">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="Y9" s="0" t="n">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="Z9" s="0" t="n">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="AA9" s="0" t="n">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="AB9" s="0" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="AC9" s="0" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="AD9" s="0" t="n">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="AE9" s="0" t="n">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AF9" s="0" t="n">
-        <v>17</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>40</v>
@@ -1243,84 +1243,84 @@
         <v>85</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="M10" s="0" t="n">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="N10" s="0" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="O10" s="0" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="P10" s="0" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="Q10" s="0" t="n">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="R10" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>598</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <v>624</v>
+      </c>
+      <c r="U10" s="0" t="n">
+        <v>1813</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <v>206649</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="X10" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="Z10" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="S10" s="0" t="n">
-        <v>268</v>
-      </c>
-      <c r="T10" s="0" t="n">
-        <v>459</v>
-      </c>
-      <c r="U10" s="0" t="n">
-        <v>1172</v>
-      </c>
-      <c r="V10" s="0" t="n">
-        <v>277687</v>
-      </c>
-      <c r="W10" s="0" t="n">
+      <c r="AA10" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB10" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="X10" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="Y10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z10" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="AA10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB10" s="0" t="n">
-        <v>32</v>
-      </c>
       <c r="AC10" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE10" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="AF10" s="0" t="n">
         <v>19</v>
-      </c>
-      <c r="AD10" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="AE10" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="AF10" s="0" t="n">
-        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>41</v>
@@ -1371,49 +1371,49 @@
         <v>40</v>
       </c>
       <c r="R11" s="0" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S11" s="0" t="n">
-        <v>805</v>
+        <v>503</v>
       </c>
       <c r="T11" s="0" t="n">
-        <v>1466</v>
+        <v>572</v>
       </c>
       <c r="U11" s="0" t="n">
-        <v>2504</v>
+        <v>2971</v>
       </c>
       <c r="V11" s="0" t="n">
-        <v>6484</v>
+        <v>204166</v>
       </c>
       <c r="W11" s="0" t="n">
         <v>27</v>
       </c>
       <c r="X11" s="0" t="n">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="Y11" s="0" t="n">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="Z11" s="0" t="n">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="AA11" s="0" t="n">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="AB11" s="0" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AC11" s="0" t="n">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="AD11" s="0" t="n">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="AE11" s="0" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="AF11" s="0" t="n">
-        <v>109</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1439,7 +1439,7 @@
         <v>85</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>1</v>
@@ -1451,10 +1451,10 @@
         <v>1</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>39</v>
@@ -1466,25 +1466,25 @@
         <v>39</v>
       </c>
       <c r="Q12" s="0" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="R12" s="0" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="S12" s="0" t="n">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="T12" s="0" t="n">
-        <v>476</v>
+        <v>322</v>
       </c>
       <c r="U12" s="0" t="n">
-        <v>1039</v>
+        <v>1454</v>
       </c>
       <c r="V12" s="0" t="n">
-        <v>811</v>
+        <v>757</v>
       </c>
       <c r="W12" s="0" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="X12" s="0" t="n">
         <v>15</v>
@@ -1493,7 +1493,7 @@
         <v>11</v>
       </c>
       <c r="Z12" s="0" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AA12" s="0" t="n">
         <v>4</v>
@@ -1502,21 +1502,21 @@
         <v>27</v>
       </c>
       <c r="AC12" s="0" t="n">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AD12" s="0" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="AE12" s="0" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AF12" s="0" t="n">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>43</v>
@@ -1537,84 +1537,84 @@
         <v>85</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="M13" s="0" t="n">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="O13" s="0" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="P13" s="0" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="Q13" s="0" t="n">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="R13" s="0" t="n">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="S13" s="0" t="n">
-        <v>512</v>
+        <v>352</v>
       </c>
       <c r="T13" s="0" t="n">
-        <v>779</v>
+        <v>465</v>
       </c>
       <c r="U13" s="0" t="n">
-        <v>1512</v>
+        <v>1640</v>
       </c>
       <c r="V13" s="0" t="n">
-        <v>208656</v>
+        <v>294052</v>
       </c>
       <c r="W13" s="0" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="X13" s="0" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="Y13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z13" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB13" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="Z13" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="AA13" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="AB13" s="0" t="n">
-        <v>27</v>
-      </c>
       <c r="AC13" s="0" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AD13" s="0" t="n">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="AE13" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AF13" s="0" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>44</v>
@@ -1635,84 +1635,84 @@
         <v>85</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="M14" s="0" t="n">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="N14" s="0" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="O14" s="0" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="P14" s="0" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="Q14" s="0" t="n">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="R14" s="0" t="n">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="S14" s="0" t="n">
-        <v>698</v>
+        <v>675</v>
       </c>
       <c r="T14" s="0" t="n">
-        <v>626</v>
+        <v>584</v>
       </c>
       <c r="U14" s="0" t="n">
-        <v>1982</v>
+        <v>1722</v>
       </c>
       <c r="V14" s="0" t="n">
-        <v>241860</v>
+        <v>198938</v>
       </c>
       <c r="W14" s="0" t="n">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="X14" s="0" t="n">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="Y14" s="0" t="n">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="Z14" s="0" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="AA14" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AB14" s="0" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="AC14" s="0" t="n">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="AD14" s="0" t="n">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="AE14" s="0" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="AF14" s="0" t="n">
-        <v>153</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>45</v>
@@ -1733,79 +1733,79 @@
         <v>85</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="M15" s="0" t="n">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="N15" s="0" t="n">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="O15" s="0" t="n">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="P15" s="0" t="n">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="Q15" s="0" t="n">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="R15" s="0" t="n">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="S15" s="0" t="n">
-        <v>214</v>
+        <v>861</v>
       </c>
       <c r="T15" s="0" t="n">
-        <v>431</v>
+        <v>1738</v>
       </c>
       <c r="U15" s="0" t="n">
-        <v>1119</v>
+        <v>2064</v>
       </c>
       <c r="V15" s="0" t="n">
-        <v>752</v>
+        <v>1598</v>
       </c>
       <c r="W15" s="0" t="n">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="X15" s="0" t="n">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="Y15" s="0" t="n">
-        <v>8</v>
+        <v>124</v>
       </c>
       <c r="Z15" s="0" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="AA15" s="0" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="AB15" s="0" t="n">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="AC15" s="0" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="AD15" s="0" t="n">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AE15" s="0" t="n">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="AF15" s="0" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,49 +1861,49 @@
         <v>85</v>
       </c>
       <c r="R16" s="0" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="S16" s="0" t="n">
-        <v>654</v>
+        <v>433</v>
       </c>
       <c r="T16" s="0" t="n">
-        <v>686</v>
+        <v>665</v>
       </c>
       <c r="U16" s="0" t="n">
-        <v>1490</v>
+        <v>2905</v>
       </c>
       <c r="V16" s="0" t="n">
-        <v>218306</v>
+        <v>202252</v>
       </c>
       <c r="W16" s="0" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="X16" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y16" s="0" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Z16" s="0" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="AA16" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB16" s="0" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AC16" s="0" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="AD16" s="0" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="AE16" s="0" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="AF16" s="0" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1959,49 +1959,49 @@
         <v>40</v>
       </c>
       <c r="R17" s="0" t="n">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="S17" s="0" t="n">
-        <v>458</v>
+        <v>439</v>
       </c>
       <c r="T17" s="0" t="n">
-        <v>695</v>
+        <v>543</v>
       </c>
       <c r="U17" s="0" t="n">
-        <v>1446</v>
+        <v>1685</v>
       </c>
       <c r="V17" s="0" t="n">
-        <v>223406</v>
+        <v>204830</v>
       </c>
       <c r="W17" s="0" t="n">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="X17" s="0" t="n">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="Y17" s="0" t="n">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="Z17" s="0" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="AA17" s="0" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="AB17" s="0" t="n">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="AC17" s="0" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="AD17" s="0" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="AE17" s="0" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AF17" s="0" t="n">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2027,7 +2027,7 @@
         <v>85</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>1</v>
@@ -2039,10 +2039,10 @@
         <v>1</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M18" s="0" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>39</v>
@@ -2054,57 +2054,57 @@
         <v>39</v>
       </c>
       <c r="Q18" s="0" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="R18" s="0" t="n">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="S18" s="0" t="n">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="T18" s="0" t="n">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="U18" s="0" t="n">
-        <v>1218</v>
+        <v>1239</v>
       </c>
       <c r="V18" s="0" t="n">
-        <v>1150</v>
+        <v>1019</v>
       </c>
       <c r="W18" s="0" t="n">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="X18" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Y18" s="0" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="Z18" s="0" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AA18" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AB18" s="0" t="n">
-        <v>135</v>
+        <v>26</v>
       </c>
       <c r="AC18" s="0" t="n">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="AD18" s="0" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="AE18" s="0" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AF18" s="0" t="n">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>49</v>
@@ -2125,84 +2125,84 @@
         <v>85</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="K19" s="0" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="L19" s="0" t="n">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="M19" s="0" t="n">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="N19" s="0" t="n">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="O19" s="0" t="n">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="P19" s="0" t="n">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="Q19" s="0" t="n">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="R19" s="0" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="S19" s="0" t="n">
-        <v>830</v>
+        <v>315</v>
       </c>
       <c r="T19" s="0" t="n">
-        <v>1461</v>
+        <v>376</v>
       </c>
       <c r="U19" s="0" t="n">
-        <v>2170</v>
+        <v>1640</v>
       </c>
       <c r="V19" s="0" t="n">
-        <v>2366</v>
+        <v>268328</v>
       </c>
       <c r="W19" s="0" t="n">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="X19" s="0" t="n">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="Y19" s="0" t="n">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="Z19" s="0" t="n">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="AA19" s="0" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="AB19" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="AC19" s="0" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AD19" s="0" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="AE19" s="0" t="n">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="AF19" s="0" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>50</v>
@@ -2211,96 +2211,96 @@
         <v>85</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>85</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="L20" s="0" t="n">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="M20" s="0" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="N20" s="0" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="O20" s="0" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="P20" s="0" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="Q20" s="0" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="R20" s="0" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="S20" s="0" t="n">
-        <v>784</v>
+        <v>475</v>
       </c>
       <c r="T20" s="0" t="n">
-        <v>1179</v>
+        <v>609</v>
       </c>
       <c r="U20" s="0" t="n">
-        <v>1899</v>
+        <v>1450</v>
       </c>
       <c r="V20" s="0" t="n">
-        <v>1737</v>
+        <v>211291</v>
       </c>
       <c r="W20" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="X20" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="Y20" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="Z20" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA20" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="X20" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="Y20" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="Z20" s="0" t="n">
+      <c r="AB20" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="AA20" s="0" t="n">
+      <c r="AC20" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="AB20" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="AC20" s="0" t="n">
-        <v>28</v>
-      </c>
       <c r="AD20" s="0" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="AE20" s="0" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AF20" s="0" t="n">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>51</v>
@@ -2321,84 +2321,84 @@
         <v>85</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="K21" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="L21" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="M21" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="N21" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="O21" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="P21" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="Q21" s="0" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="R21" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="S21" s="0" t="n">
+        <v>609</v>
+      </c>
+      <c r="T21" s="0" t="n">
+        <v>1329</v>
+      </c>
+      <c r="U21" s="0" t="n">
+        <v>1929</v>
+      </c>
+      <c r="V21" s="0" t="n">
+        <v>1040</v>
+      </c>
+      <c r="W21" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="X21" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="Y21" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="S21" s="0" t="n">
-        <v>170</v>
-      </c>
-      <c r="T21" s="0" t="n">
-        <v>368</v>
-      </c>
-      <c r="U21" s="0" t="n">
-        <v>892</v>
-      </c>
-      <c r="V21" s="0" t="n">
-        <v>507</v>
-      </c>
-      <c r="W21" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="X21" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="Y21" s="0" t="n">
-        <v>6</v>
-      </c>
       <c r="Z21" s="0" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="AA21" s="0" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="AB21" s="0" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AC21" s="0" t="n">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="AD21" s="0" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AE21" s="0" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="AF21" s="0" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>52</v>
@@ -2449,54 +2449,54 @@
         <v>40</v>
       </c>
       <c r="R22" s="0" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="S22" s="0" t="n">
-        <v>379</v>
+        <v>507</v>
       </c>
       <c r="T22" s="0" t="n">
-        <v>801</v>
+        <v>491</v>
       </c>
       <c r="U22" s="0" t="n">
-        <v>1198</v>
+        <v>4922</v>
       </c>
       <c r="V22" s="0" t="n">
-        <v>217575</v>
+        <v>207142</v>
       </c>
       <c r="W22" s="0" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="X22" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="Y22" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="Z22" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA22" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB22" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC22" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD22" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AE22" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="AF22" s="0" t="n">
         <v>14</v>
-      </c>
-      <c r="Y22" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="Z22" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="AA22" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="AB22" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="AC22" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="AD22" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="AE22" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="AF22" s="0" t="n">
-        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>53</v>
@@ -2550,51 +2550,51 @@
         <v>36</v>
       </c>
       <c r="S23" s="0" t="n">
-        <v>629</v>
+        <v>590</v>
       </c>
       <c r="T23" s="0" t="n">
-        <v>1418</v>
+        <v>449</v>
       </c>
       <c r="U23" s="0" t="n">
-        <v>1819</v>
+        <v>1457</v>
       </c>
       <c r="V23" s="0" t="n">
-        <v>1302</v>
+        <v>205592</v>
       </c>
       <c r="W23" s="0" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="X23" s="0" t="n">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="Y23" s="0" t="n">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="Z23" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA23" s="0" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AB23" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC23" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="AC23" s="0" t="n">
-        <v>19</v>
-      </c>
       <c r="AD23" s="0" t="n">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="AE23" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AF23" s="0" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>54</v>
@@ -2615,79 +2615,79 @@
         <v>85</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="I24" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="K24" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="L24" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="M24" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="N24" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="O24" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="P24" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Q24" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="R24" s="0" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="S24" s="0" t="n">
-        <v>638</v>
+        <v>170</v>
       </c>
       <c r="T24" s="0" t="n">
-        <v>916</v>
+        <v>209</v>
       </c>
       <c r="U24" s="0" t="n">
-        <v>2060</v>
+        <v>1850</v>
       </c>
       <c r="V24" s="0" t="n">
-        <v>1192</v>
+        <v>493</v>
       </c>
       <c r="W24" s="0" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="X24" s="0" t="n">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="Y24" s="0" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="Z24" s="0" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AA24" s="0" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="AB24" s="0" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AC24" s="0" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="AD24" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="AE24" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="AE24" s="0" t="n">
-        <v>10</v>
-      </c>
       <c r="AF24" s="0" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2743,46 +2743,46 @@
         <v>84</v>
       </c>
       <c r="R25" s="0" t="n">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="S25" s="0" t="n">
-        <v>253</v>
+        <v>218</v>
       </c>
       <c r="T25" s="0" t="n">
-        <v>340</v>
+        <v>294</v>
       </c>
       <c r="U25" s="0" t="n">
-        <v>1211</v>
+        <v>1492</v>
       </c>
       <c r="V25" s="0" t="n">
-        <v>288653</v>
+        <v>274563</v>
       </c>
       <c r="W25" s="0" t="n">
         <v>21</v>
       </c>
       <c r="X25" s="0" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Y25" s="0" t="n">
         <v>5</v>
       </c>
       <c r="Z25" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AA25" s="0" t="n">
         <v>3</v>
       </c>
       <c r="AB25" s="0" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AC25" s="0" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="AD25" s="0" t="n">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="AE25" s="0" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="AF25" s="0" t="n">
         <v>12</v>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>56</v>
@@ -2841,54 +2841,54 @@
         <v>40</v>
       </c>
       <c r="R26" s="0" t="n">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="S26" s="0" t="n">
-        <v>417</v>
+        <v>203</v>
       </c>
       <c r="T26" s="0" t="n">
-        <v>441</v>
+        <v>194</v>
       </c>
       <c r="U26" s="0" t="n">
-        <v>1909</v>
+        <v>723</v>
       </c>
       <c r="V26" s="0" t="n">
-        <v>225018</v>
+        <v>155555</v>
       </c>
       <c r="W26" s="0" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="X26" s="0" t="n">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="Y26" s="0" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="Z26" s="0" t="n">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="AA26" s="0" t="n">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="AB26" s="0" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="AC26" s="0" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AD26" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AE26" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AF26" s="0" t="n">
         <v>14</v>
-      </c>
-      <c r="AF26" s="0" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>57</v>
@@ -2939,28 +2939,28 @@
         <v>40</v>
       </c>
       <c r="R27" s="0" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="S27" s="0" t="n">
-        <v>208</v>
+        <v>424</v>
       </c>
       <c r="T27" s="0" t="n">
-        <v>216</v>
+        <v>637</v>
       </c>
       <c r="U27" s="0" t="n">
-        <v>752</v>
+        <v>1371</v>
       </c>
       <c r="V27" s="0" t="n">
-        <v>154730</v>
+        <v>903</v>
       </c>
       <c r="W27" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="X27" s="0" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="Y27" s="0" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="Z27" s="0" t="n">
         <v>12</v>
@@ -2972,21 +2972,21 @@
         <v>27</v>
       </c>
       <c r="AC27" s="0" t="n">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="AD27" s="0" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="AE27" s="0" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="AF27" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>58</v>
@@ -3037,46 +3037,46 @@
         <v>40</v>
       </c>
       <c r="R28" s="0" t="n">
-        <v>202</v>
+        <v>24</v>
       </c>
       <c r="S28" s="0" t="n">
-        <v>421</v>
+        <v>214</v>
       </c>
       <c r="T28" s="0" t="n">
-        <v>652</v>
+        <v>212</v>
       </c>
       <c r="U28" s="0" t="n">
-        <v>1913</v>
+        <v>830</v>
       </c>
       <c r="V28" s="0" t="n">
-        <v>1065</v>
+        <v>156204</v>
       </c>
       <c r="W28" s="0" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="X28" s="0" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="Y28" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Z28" s="0" t="n">
         <v>12</v>
-      </c>
-      <c r="Z28" s="0" t="n">
-        <v>16</v>
       </c>
       <c r="AA28" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AB28" s="0" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="AC28" s="0" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AD28" s="0" t="n">
         <v>11</v>
       </c>
       <c r="AE28" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AF28" s="0" t="n">
         <v>15</v>
@@ -3084,7 +3084,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>59</v>
@@ -3135,54 +3135,54 @@
         <v>40</v>
       </c>
       <c r="R29" s="0" t="n">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="S29" s="0" t="n">
-        <v>369</v>
+        <v>227</v>
       </c>
       <c r="T29" s="0" t="n">
-        <v>595</v>
+        <v>187</v>
       </c>
       <c r="U29" s="0" t="n">
-        <v>1216</v>
+        <v>715</v>
       </c>
       <c r="V29" s="0" t="n">
-        <v>890</v>
+        <v>150270</v>
       </c>
       <c r="W29" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="X29" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="Y29" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="Y29" s="0" t="n">
-        <v>12</v>
-      </c>
       <c r="Z29" s="0" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="AA29" s="0" t="n">
         <v>9</v>
       </c>
       <c r="AB29" s="0" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AC29" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD29" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="AD29" s="0" t="n">
-        <v>11</v>
-      </c>
       <c r="AE29" s="0" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AF29" s="0" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>60</v>
@@ -3203,84 +3203,84 @@
         <v>85</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="I30" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="J30" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="K30" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="L30" s="0" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="M30" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="N30" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="O30" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="P30" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Q30" s="0" t="n">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="R30" s="0" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S30" s="0" t="n">
-        <v>204</v>
+        <v>15</v>
       </c>
       <c r="T30" s="0" t="n">
-        <v>325</v>
+        <v>17</v>
       </c>
       <c r="U30" s="0" t="n">
-        <v>772</v>
+        <v>445</v>
       </c>
       <c r="V30" s="0" t="n">
-        <v>158592</v>
+        <v>420</v>
       </c>
       <c r="W30" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="X30" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z30" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA30" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB30" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC30" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="AD30" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="AE30" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AF30" s="0" t="n">
         <v>11</v>
-      </c>
-      <c r="Y30" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="Z30" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="AA30" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="AB30" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="AC30" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="AD30" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="AE30" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="AF30" s="0" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>61</v>
@@ -3331,28 +3331,28 @@
         <v>84</v>
       </c>
       <c r="R31" s="0" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="S31" s="0" t="n">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="T31" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="U31" s="0" t="n">
+        <v>689</v>
+      </c>
+      <c r="V31" s="0" t="n">
+        <v>209513</v>
+      </c>
+      <c r="W31" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="U31" s="0" t="n">
-        <v>564</v>
-      </c>
-      <c r="V31" s="0" t="n">
-        <v>447</v>
-      </c>
-      <c r="W31" s="0" t="n">
-        <v>23</v>
-      </c>
       <c r="X31" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y31" s="0" t="n">
         <v>4</v>
-      </c>
-      <c r="Y31" s="0" t="n">
-        <v>7</v>
       </c>
       <c r="Z31" s="0" t="n">
         <v>4</v>
@@ -3361,19 +3361,19 @@
         <v>3</v>
       </c>
       <c r="AB31" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AC31" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD31" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE31" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AD31" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="AE31" s="0" t="n">
-        <v>7</v>
-      </c>
       <c r="AF31" s="0" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>